<commit_message>
Update Total Address Growth Rate.xlsx
</commit_message>
<xml_diff>
--- a/Output/Total Address Growth Rate.xlsx
+++ b/Output/Total Address Growth Rate.xlsx
@@ -32,37 +32,37 @@
     <t xml:space="preserve">LIC selected</t>
   </si>
   <si>
-    <t xml:space="preserve">2014-09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015-09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016-09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020-09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021-09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-09</t>
+    <t xml:space="preserve">2014-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-12</t>
   </si>
   <si>
     <t xml:space="preserve">Pre-OZs Avg. Annual Growth</t>
@@ -425,19 +425,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>15803506</v>
+        <v>15837972</v>
       </c>
       <c r="C2" t="n">
-        <v>227030</v>
+        <v>227858</v>
       </c>
       <c r="D2" t="n">
-        <v>55062798</v>
+        <v>55198614</v>
       </c>
       <c r="E2" t="n">
-        <v>33946627</v>
+        <v>33993547</v>
       </c>
       <c r="F2" t="n">
-        <v>10670061</v>
+        <v>10686288</v>
       </c>
     </row>
     <row r="3">
@@ -445,19 +445,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>15960120</v>
+        <v>15997388</v>
       </c>
       <c r="C3" t="n">
-        <v>230742</v>
+        <v>231370</v>
       </c>
       <c r="D3" t="n">
-        <v>55712041</v>
+        <v>55862465</v>
       </c>
       <c r="E3" t="n">
-        <v>34134976</v>
+        <v>34178087</v>
       </c>
       <c r="F3" t="n">
-        <v>10741003</v>
+        <v>10758850</v>
       </c>
     </row>
     <row r="4">
@@ -465,19 +465,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>16110051</v>
+        <v>16150496</v>
       </c>
       <c r="C4" t="n">
-        <v>233418</v>
+        <v>234275</v>
       </c>
       <c r="D4" t="n">
-        <v>56370128</v>
+        <v>56532151</v>
       </c>
       <c r="E4" t="n">
-        <v>34322254</v>
+        <v>34370085</v>
       </c>
       <c r="F4" t="n">
-        <v>10808051</v>
+        <v>10829217</v>
       </c>
     </row>
     <row r="5">
@@ -485,19 +485,19 @@
         <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>16259861</v>
+        <v>16295265</v>
       </c>
       <c r="C5" t="n">
-        <v>236255</v>
+        <v>236703</v>
       </c>
       <c r="D5" t="n">
-        <v>57078682</v>
+        <v>57232615</v>
       </c>
       <c r="E5" t="n">
-        <v>34515198</v>
+        <v>34559337</v>
       </c>
       <c r="F5" t="n">
-        <v>10876607</v>
+        <v>10891399</v>
       </c>
     </row>
     <row r="6">
@@ -505,19 +505,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="n">
-        <v>16437369</v>
+        <v>16475801</v>
       </c>
       <c r="C6" t="n">
-        <v>238980</v>
+        <v>239501</v>
       </c>
       <c r="D6" t="n">
-        <v>57816819</v>
+        <v>57977671</v>
       </c>
       <c r="E6" t="n">
-        <v>34719942</v>
+        <v>34766030</v>
       </c>
       <c r="F6" t="n">
-        <v>10956502</v>
+        <v>10971268</v>
       </c>
     </row>
     <row r="7">
@@ -525,19 +525,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="n">
-        <v>16616200</v>
+        <v>16658691</v>
       </c>
       <c r="C7" t="n">
-        <v>241444</v>
+        <v>242324</v>
       </c>
       <c r="D7" t="n">
-        <v>58582032</v>
+        <v>58761104</v>
       </c>
       <c r="E7" t="n">
-        <v>34948131</v>
+        <v>35004427</v>
       </c>
       <c r="F7" t="n">
-        <v>11040777</v>
+        <v>11064101</v>
       </c>
     </row>
     <row r="8">
@@ -545,19 +545,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="n">
-        <v>16792486</v>
+        <v>16839617</v>
       </c>
       <c r="C8" t="n">
-        <v>244689</v>
+        <v>245594</v>
       </c>
       <c r="D8" t="n">
-        <v>59313397</v>
+        <v>59499758</v>
       </c>
       <c r="E8" t="n">
-        <v>35146197</v>
+        <v>35205576</v>
       </c>
       <c r="F8" t="n">
-        <v>11120071</v>
+        <v>11142274</v>
       </c>
     </row>
     <row r="9">
@@ -565,19 +565,19 @@
         <v>13</v>
       </c>
       <c r="B9" t="n">
-        <v>16994655</v>
+        <v>17042979</v>
       </c>
       <c r="C9" t="n">
-        <v>248863</v>
+        <v>249416</v>
       </c>
       <c r="D9" t="n">
-        <v>60178302</v>
+        <v>60393769</v>
       </c>
       <c r="E9" t="n">
-        <v>35393243</v>
+        <v>35446022</v>
       </c>
       <c r="F9" t="n">
-        <v>11229007</v>
+        <v>11261191</v>
       </c>
     </row>
     <row r="10">
@@ -585,19 +585,19 @@
         <v>14</v>
       </c>
       <c r="B10" t="n">
-        <v>17216365</v>
+        <v>17269164</v>
       </c>
       <c r="C10" t="n">
-        <v>253408</v>
+        <v>254024</v>
       </c>
       <c r="D10" t="n">
-        <v>61059978</v>
+        <v>61238550</v>
       </c>
       <c r="E10" t="n">
-        <v>35687306</v>
+        <v>35754594</v>
       </c>
       <c r="F10" t="n">
-        <v>11368159</v>
+        <v>11400953</v>
       </c>
     </row>
     <row r="11">
@@ -605,19 +605,19 @@
         <v>15</v>
       </c>
       <c r="B11" t="n">
-        <v>17394800</v>
+        <v>17461826</v>
       </c>
       <c r="C11" t="n">
-        <v>256691</v>
+        <v>259603</v>
       </c>
       <c r="D11" t="n">
-        <v>61765087</v>
+        <v>62003759</v>
       </c>
       <c r="E11" t="n">
-        <v>35919647</v>
+        <v>35978294</v>
       </c>
       <c r="F11" t="n">
-        <v>11485528</v>
+        <v>11518590</v>
       </c>
     </row>
     <row r="12">
@@ -625,19 +625,19 @@
         <v>16</v>
       </c>
       <c r="B12" t="n">
-        <v>17680903</v>
+        <v>17722036</v>
       </c>
       <c r="C12" t="n">
-        <v>263739</v>
+        <v>264116</v>
       </c>
       <c r="D12" t="n">
-        <v>62780406</v>
+        <v>62933151</v>
       </c>
       <c r="E12" t="n">
-        <v>36304733</v>
+        <v>36360053</v>
       </c>
       <c r="F12" t="n">
-        <v>11692274</v>
+        <v>11717813</v>
       </c>
     </row>
     <row r="13">
@@ -645,19 +645,19 @@
         <v>17</v>
       </c>
       <c r="B13" t="n">
-        <v>1.00799658051637</v>
+        <v>1.01559122203156</v>
       </c>
       <c r="C13" t="n">
-        <v>1.2389285086471</v>
+        <v>1.23880742378265</v>
       </c>
       <c r="D13" t="n">
-        <v>1.24679939773407</v>
+        <v>1.25871901931235</v>
       </c>
       <c r="E13" t="n">
-        <v>0.583211899326659</v>
+        <v>0.587811009777879</v>
       </c>
       <c r="F13" t="n">
-        <v>0.685427091015054</v>
+        <v>0.697346427695706</v>
       </c>
     </row>
     <row r="14">
@@ -665,19 +665,19 @@
         <v>18</v>
       </c>
       <c r="B14" t="n">
-        <v>1.25012576919903</v>
+        <v>1.24533347717766</v>
       </c>
       <c r="C14" t="n">
-        <v>1.7834789518827</v>
+        <v>1.7375697148786</v>
       </c>
       <c r="D14" t="n">
-        <v>1.3940735455782</v>
+        <v>1.38137252977639</v>
       </c>
       <c r="E14" t="n">
-        <v>0.764724052376205</v>
+        <v>0.762978330759675</v>
       </c>
       <c r="F14" t="n">
-        <v>1.15390764023835</v>
+        <v>1.15525912037069</v>
       </c>
     </row>
   </sheetData>

</xml_diff>